<commit_message>
Move case_files from config.py to run.py
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -336,6 +336,22 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -398,7 +414,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-06 12:01:59</t>
+    <t>2017-10-07 02:01:04</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -434,7 +450,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-10-06 12:02:01</t>
+    <t>2017-10-07 02:01:06</t>
   </si>
   <si>
     <t>Search box</t>
@@ -476,7 +492,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-10-06 12:02:04</t>
+    <t>2017-10-07 02:01:09</t>
   </si>
   <si>
     <t>(Load the saved)</t>

</xml_diff>

<commit_message>
Add basic function for Locust load testing engine.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -28,13 +28,29 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="155">
   <si>
     <t>Run</t>
   </si>
@@ -90,7 +106,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-09 11:53:07</t>
+    <t>2017-10-09 20:45:11</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -126,7 +142,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-10-09 11:53:09</t>
+    <t>2017-10-09 20:45:16</t>
   </si>
   <si>
     <t>Search box</t>
@@ -168,7 +184,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-10-09 11:53:12</t>
+    <t>2017-10-09 20:45:19</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -321,22 +337,16 @@
     <t>get</t>
   </si>
   <si>
-    <t>https://github.com/timeline.json</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>2017-10-03 23:39:33</t>
-  </si>
-  <si>
-    <t>[Line 0] HTTPSConnectionPool(host='github.com', port=443): Read timed out. (read timeout=1.0)</t>
+    <t>https://api.github.com</t>
+  </si>
+  <si>
+    <t>2017-10-09 20:45:22</t>
   </si>
   <si>
     <t>in.text</t>
   </si>
   <si>
-    <t>message</t>
+    <t>emojis</t>
   </si>
   <si>
     <t>AT.HTTP.Get.02</t>
@@ -384,13 +394,13 @@
     <t>&lt;headers&gt;</t>
   </si>
   <si>
-    <t>2017-10-02 19:46:36</t>
+    <t>2017-10-09 20:45:23</t>
   </si>
   <si>
     <t>user-agent</t>
   </si>
   <si>
-    <t>my-app/0.0.1</t>
+    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/61.0.3163.100 Safari/537.36</t>
   </si>
   <si>
     <t>&lt;/headers&gt;</t>
@@ -399,22 +409,37 @@
     <t>&lt;params&gt;</t>
   </si>
   <si>
-    <t>key1</t>
-  </si>
-  <si>
-    <t>value1</t>
-  </si>
-  <si>
-    <t>key2</t>
-  </si>
-  <si>
-    <t>value2</t>
+    <t>name</t>
   </si>
   <si>
     <t>&lt;/params&gt;</t>
   </si>
   <si>
-    <t>zzz</t>
+    <t>https://www.v2ex.com/api/nodes/show.json</t>
+  </si>
+  <si>
+    <t>log.text</t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.04</t>
+  </si>
+  <si>
+    <t>2017-10-09 20:45:25</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>https://api.github.com/repos/txels/ddt/issues</t>
+  </si>
+  <si>
+    <t>Add zeros</t>
   </si>
   <si>
     <t>AT.MYSQL.Select.01</t>
@@ -445,6 +470,30 @@
   </si>
   <si>
     <t>fetchmany.5</t>
+  </si>
+  <si>
+    <t>AT.Locust.01</t>
+  </si>
+  <si>
+    <t>locust</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>2017-10-09 20:45:26</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>LocustExample.py</t>
   </si>
   <si>
     <t>Locate/Encapsulate</t>
@@ -561,7 +610,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -581,6 +630,9 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -859,10 +911,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="A10" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView showRuler="0" tabSelected="1" topLeftCell="A54" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -875,12 +927,12 @@
     <col customWidth="1" max="6" min="6" style="7" width="11"/>
     <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="38.1640625"/>
     <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="16.6640625"/>
-    <col customWidth="1" max="9" min="9" style="7" width="31.6640625"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="7" width="40"/>
     <col customWidth="1" max="10" min="10" style="7" width="8.33203125"/>
     <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
     <col bestFit="1" customWidth="1" max="12" min="12" style="7" width="80.1640625"/>
-    <col customWidth="1" max="32" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="33" style="7" width="10.83203125"/>
+    <col customWidth="1" max="34" min="13" style="7" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="35" style="7" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:12">
@@ -1100,7 +1152,7 @@
       <c r="K10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="3" t="s"/>
+      <c r="L10" s="3" t="n"/>
     </row>
     <row r="11" spans="1:12">
       <c r="D11" s="7" t="s">
@@ -1468,7 +1520,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="2" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>91</v>
@@ -1489,21 +1541,19 @@
         <v>95</v>
       </c>
       <c r="J32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="L32" s="3" t="n"/>
     </row>
     <row r="33" spans="1:12">
       <c r="H33" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1511,7 +1561,7 @@
         <v>48</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>92</v>
@@ -1521,10 +1571,10 @@
         <v>93</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H34" s="3" t="n"/>
       <c r="I34" s="3" t="n"/>
@@ -1532,21 +1582,21 @@
         <v>17</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L34" s="3" t="n"/>
     </row>
     <row r="35" spans="1:12">
       <c r="F35" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="F36" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G36" s="7" t="n">
         <v>2</v>
@@ -1557,7 +1607,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="H37" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I37" s="7" t="n">
         <v>200</v>
@@ -1565,7 +1615,7 @@
     </row>
     <row r="38" spans="1:12">
       <c r="H38" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I38" s="7" t="b">
         <v>1</v>
@@ -1573,26 +1623,26 @@
     </row>
     <row r="39" spans="1:12">
       <c r="H39" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="H40" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>92</v>
@@ -1602,7 +1652,7 @@
         <v>93</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G41" s="2" t="n"/>
       <c r="H41" s="3" t="n"/>
@@ -1611,154 +1661,287 @@
         <v>17</v>
       </c>
       <c r="K41" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L41" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="18" r="42" spans="1:12">
+      <c r="F42" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="L41" s="3" t="n"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="F42" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="F43" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="F44" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="F45" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="F46" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="F47" s="7" t="s">
-        <v>125</v>
+        <v>105</v>
+      </c>
+      <c r="G47" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="F48" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" s="7" t="n">
-        <v>5</v>
-      </c>
       <c r="H48" s="4" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
     </row>
     <row customHeight="1" ht="19" r="49" spans="1:12">
       <c r="H49" s="7" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="H50" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="I50" s="7" t="s">
+      <c r="A50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="3" t="n"/>
+      <c r="E50" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="2" t="n"/>
+      <c r="H50" s="3" t="n"/>
+      <c r="I50" s="3" t="n"/>
+      <c r="J50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L50" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="18" r="51" spans="1:12">
+      <c r="F51" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="F52" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="F53" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="F54" s="7" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="2" t="s">
+      <c r="G54" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="F55" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="F56" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G56" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="19" r="57" spans="1:12">
+      <c r="H57" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D51" s="3" t="n"/>
-      <c r="E51" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F51" s="3" t="n"/>
-      <c r="G51" s="3" t="n"/>
-      <c r="H51" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="D58" s="3" t="n"/>
+      <c r="E58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F58" s="3" t="n"/>
+      <c r="G58" s="3" t="n"/>
+      <c r="H58" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J58" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L51" s="3" t="n"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="H52" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="H53" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I53" s="7" t="s">
+      <c r="K58" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L58" s="3" t="n"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="H59" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="H60" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="H61" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="H62" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="H63" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="H64" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="H65" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="H54" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="H55" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="I55" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="H56" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="H57" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="I57" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="H58" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I58" s="7" t="s">
-        <v>135</v>
+      <c r="D66" s="3" t="n"/>
+      <c r="E66" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G66" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H66" s="3" t="n"/>
+      <c r="I66" s="2" t="n"/>
+      <c r="J66" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L66" s="3" t="s"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="F67" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="F68" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" s="7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="F69" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1792,8 +1975,8 @@
     <col bestFit="1" customWidth="1" max="10" min="10" style="7" width="8.1640625"/>
     <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
     <col customWidth="1" max="12" min="12" style="7" width="31.83203125"/>
-    <col customWidth="1" max="31" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="32" style="7" width="10.83203125"/>
+    <col customWidth="1" max="33" min="13" style="7" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="34" style="7" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:12">
@@ -1813,13 +1996,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1839,14 +2022,14 @@
         <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D2" s="3" t="n"/>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
@@ -1863,10 +2046,10 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
@@ -1894,10 +2077,10 @@
         <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">

</xml_diff>

<commit_message>
Add background support for Locust load testing engine.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -44,6 +44,80 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -106,7 +180,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:11</t>
+    <t>2017-10-09 22:02:09</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
@@ -142,7 +216,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:16</t>
+    <t>2017-10-09 22:02:12</t>
   </si>
   <si>
     <t>Search box</t>
@@ -184,7 +258,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:19</t>
+    <t>2017-10-09 22:02:14</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -340,7 +414,7 @@
     <t>https://api.github.com</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:22</t>
+    <t>2017-10-09 22:02:18</t>
   </si>
   <si>
     <t>in.text</t>
@@ -394,7 +468,7 @@
     <t>&lt;headers&gt;</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:23</t>
+    <t>2017-10-09 22:02:19</t>
   </si>
   <si>
     <t>user-agent</t>
@@ -427,7 +501,7 @@
     <t>AT.HTTP.Get.04</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:25</t>
+    <t>2017-10-09 22:02:20</t>
   </si>
   <si>
     <t>state</t>
@@ -481,7 +555,7 @@
     <t>client</t>
   </si>
   <si>
-    <t>2017-10-09 20:45:26</t>
+    <t>2017-10-09 22:02:22</t>
   </si>
   <si>
     <t>rate</t>

</xml_diff>

<commit_message>
Fix example to avoid exceeding the limit of github.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -1,130 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/TestCases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="8280" yWindow="460" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$40</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="157">
   <si>
     <t>Run</t>
   </si>
@@ -474,9 +382,6 @@
     <t>user-agent</t>
   </si>
   <si>
-    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/61.0.3163.100 Safari/537.36</t>
-  </si>
-  <si>
     <t>&lt;/headers&gt;</t>
   </si>
   <si>
@@ -489,174 +394,192 @@
     <t>&lt;/params&gt;</t>
   </si>
   <si>
+    <t>log.text</t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.04</t>
+  </si>
+  <si>
+    <t>2017-10-09 22:02:20</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Add zeros</t>
+  </si>
+  <si>
+    <t>AT.MYSQL.Select.01</t>
+  </si>
+  <si>
+    <t>mysql</t>
+  </si>
+  <si>
+    <t>fetchone</t>
+  </si>
+  <si>
+    <t>SELECT name FROM help_keyword;</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>fetchone.name</t>
+  </si>
+  <si>
+    <t>fetchall</t>
+  </si>
+  <si>
+    <t>AES_ENCRYPT</t>
+  </si>
+  <si>
+    <t>fetchmany.5</t>
+  </si>
+  <si>
+    <t>AT.Locust.01</t>
+  </si>
+  <si>
+    <t>locust</t>
+  </si>
+  <si>
+    <t>2017-10-09 22:02:22</t>
+  </si>
+  <si>
+    <t>LocustExample.py</t>
+  </si>
+  <si>
+    <t>Locate/Encapsulate</t>
+  </si>
+  <si>
+    <t>Action/Check</t>
+  </si>
+  <si>
+    <t>AT.Login.11</t>
+  </si>
+  <si>
+    <t>登录</t>
+  </si>
+  <si>
+    <t>uI</t>
+  </si>
+  <si>
+    <t>AT.Login.12</t>
+  </si>
+  <si>
+    <t>AT.Login.13</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RATE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB Test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load Test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (MSIE 10.0; Windows NT 6.1; Trident/5.0)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>https://www.v2ex.com/api/nodes/show.json</t>
-  </si>
-  <si>
-    <t>log.text</t>
-  </si>
-  <si>
-    <t>Django</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.04</t>
-  </si>
-  <si>
-    <t>2017-10-09 22:02:20</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>https://api.github.com/repos/txels/ddt/issues</t>
-  </si>
-  <si>
-    <t>Add zeros</t>
-  </si>
-  <si>
-    <t>AT.MYSQL.Select.01</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>mysql</t>
-  </si>
-  <si>
-    <t>fetchone</t>
-  </si>
-  <si>
-    <t>SELECT name FROM help_keyword;</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>fetchone.name</t>
-  </si>
-  <si>
-    <t>fetchall</t>
-  </si>
-  <si>
-    <t>AES_ENCRYPT</t>
-  </si>
-  <si>
-    <t>fetchmany.5</t>
-  </si>
-  <si>
-    <t>AT.Locust.01</t>
-  </si>
-  <si>
-    <t>locust</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>2017-10-09 22:02:22</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>host</t>
-  </si>
-  <si>
-    <t>LocustExample.py</t>
-  </si>
-  <si>
-    <t>Locate/Encapsulate</t>
-  </si>
-  <si>
-    <t>Action/Check</t>
-  </si>
-  <si>
-    <t>AT.Login.11</t>
-  </si>
-  <si>
-    <t>登录</t>
-  </si>
-  <si>
-    <t>uI</t>
-  </si>
-  <si>
-    <t>AT.Login.12</t>
-  </si>
-  <si>
-    <t>AT.Login.13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Safari/604.1.38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="11"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="DengXian"/>
+      <family val="4"/>
       <charset val="134"/>
-      <family val="4"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,41 +603,47 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
-    <cellStyle builtinId="8" hidden="1" name="超链接" xfId="1"/>
-    <cellStyle builtinId="9" hidden="1" name="已访问的超链接" xfId="2"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -980,36 +909,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="A54" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="7" width="6.5"/>
-    <col customWidth="1" max="2" min="2" style="7" width="18.1640625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="7" width="21.33203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="7" width="18"/>
-    <col customWidth="1" max="5" min="5" style="7" width="9"/>
-    <col customWidth="1" max="6" min="6" style="7" width="11"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="38.1640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="16.6640625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="7" width="40"/>
-    <col customWidth="1" max="10" min="10" style="7" width="8.33203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="7" width="80.1640625"/>
-    <col customWidth="1" max="34" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="35" style="7" width="10.83203125"/>
+    <col min="1" max="1" width="6.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11" style="7" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="35" width="10.83203125" style="7" customWidth="1"/>
+    <col min="36" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1063,21 +988,21 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1093,8 +1018,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1107,14 +1032,14 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1122,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1138,8 +1063,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1152,9 +1077,9 @@
       <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="3" t="n"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D7" s="7" t="s">
         <v>31</v>
       </c>
@@ -1171,7 +1096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1182,7 +1107,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="7" t="s">
         <v>39</v>
       </c>
@@ -1196,7 +1121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1212,8 +1137,8 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1226,9 +1151,9 @@
       <c r="K10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="3" t="n"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="7" t="s">
         <v>45</v>
       </c>
@@ -1245,15 +1170,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F13" s="7" t="s">
         <v>32</v>
       </c>
@@ -1264,7 +1189,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -1280,8 +1205,8 @@
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1294,9 +1219,9 @@
       <c r="K14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="3" t="n"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="7" t="s">
         <v>54</v>
       </c>
@@ -1313,7 +1238,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="7" t="s">
         <v>58</v>
       </c>
@@ -1330,7 +1255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D17" s="7" t="s">
         <v>61</v>
       </c>
@@ -1343,11 +1268,11 @@
       <c r="H17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D18" s="7" t="s">
         <v>41</v>
       </c>
@@ -1355,7 +1280,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
@@ -1371,8 +1296,8 @@
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1385,9 +1310,9 @@
       <c r="K19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L19" s="3" t="n"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D20" s="7" t="s">
         <v>68</v>
       </c>
@@ -1400,11 +1325,11 @@
       <c r="H20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H21" s="7" t="s">
         <v>34</v>
       </c>
@@ -1412,7 +1337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1429,7 +1354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D23" s="7" t="s">
         <v>70</v>
       </c>
@@ -1440,7 +1365,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>48</v>
       </c>
@@ -1450,12 +1375,12 @@
       <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="3" t="n"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="3" t="n"/>
-      <c r="G24" s="3" t="n"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="2" t="s">
         <v>76</v>
       </c>
@@ -1468,9 +1393,9 @@
       <c r="K24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L24" s="3" t="n"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H25" s="7" t="s">
         <v>79</v>
       </c>
@@ -1478,7 +1403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
@@ -1488,12 +1413,12 @@
       <c r="C26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="3" t="n"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="3" t="n"/>
-      <c r="G26" s="3" t="n"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="2" t="s">
         <v>83</v>
       </c>
@@ -1506,9 +1431,9 @@
       <c r="K26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L26" s="3" t="n"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H27" s="7" t="s">
         <v>79</v>
       </c>
@@ -1516,7 +1441,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
@@ -1526,12 +1451,12 @@
       <c r="C28" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="3" t="n"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="3" t="n"/>
-      <c r="G28" s="3" t="n"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="2" t="s">
         <v>87</v>
       </c>
@@ -1544,9 +1469,9 @@
       <c r="K28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L28" s="3" t="n"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H29" s="7" t="s">
         <v>79</v>
       </c>
@@ -1554,7 +1479,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
@@ -1564,12 +1489,12 @@
       <c r="C30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="3" t="n"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="3" t="n"/>
-      <c r="G30" s="3" t="n"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="2" t="s">
         <v>90</v>
       </c>
@@ -1582,9 +1507,9 @@
       <c r="K30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L30" s="3" t="n"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H31" s="7" t="s">
         <v>79</v>
       </c>
@@ -1592,7 +1517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
@@ -1602,12 +1527,12 @@
       <c r="C32" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="3" t="n"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="3" t="n"/>
-      <c r="G32" s="3" t="n"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="2" t="s">
         <v>94</v>
       </c>
@@ -1620,9 +1545,9 @@
       <c r="K32" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L32" s="3" t="n"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H33" s="7" t="s">
         <v>97</v>
       </c>
@@ -1630,7 +1555,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
@@ -1640,7 +1565,7 @@
       <c r="C34" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="3" t="n"/>
+      <c r="D34" s="3"/>
       <c r="E34" s="2" t="s">
         <v>93</v>
       </c>
@@ -1650,17 +1575,17 @@
       <c r="G34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H34" s="3" t="n"/>
-      <c r="I34" s="3" t="n"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
       <c r="J34" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="L34" s="3" t="n"/>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F35" s="7" t="s">
         <v>103</v>
       </c>
@@ -1668,26 +1593,26 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F36" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G36" s="7" t="n">
+      <c r="G36" s="7">
         <v>2</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I37" s="7" t="n">
+      <c r="I37" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H38" s="7" t="s">
         <v>107</v>
       </c>
@@ -1695,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H39" s="7" t="s">
         <v>108</v>
       </c>
@@ -1703,7 +1628,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H40" s="7" t="s">
         <v>110</v>
       </c>
@@ -1711,7 +1636,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
@@ -1721,184 +1646,184 @@
       <c r="C41" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="3" t="n"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G41" s="2" t="n"/>
-      <c r="H41" s="3" t="n"/>
-      <c r="I41" s="3" t="n"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
       <c r="J41" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K41" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L41" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="18" r="42" spans="1:12">
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F42" s="7" t="s">
         <v>115</v>
       </c>
       <c r="G42" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F43" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
-      <c r="F43" s="7" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F44" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
-      <c r="F44" s="7" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F45" s="7" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="F45" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F46" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F47" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G47" s="7" t="n">
+      <c r="G47" s="7">
         <v>5</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>94</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H48" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="19" r="49" spans="1:12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H49" s="7" t="s">
         <v>97</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="3" t="n"/>
+      <c r="D50" s="3"/>
       <c r="E50" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G50" s="2" t="n"/>
-      <c r="H50" s="3" t="n"/>
-      <c r="I50" s="3" t="n"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
       <c r="J50" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="L50" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="18" r="51" spans="1:12">
+        <v>123</v>
+      </c>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F51" s="7" t="s">
         <v>115</v>
       </c>
       <c r="G51" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F52" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
-      <c r="F52" s="7" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F53" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
-      <c r="F53" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F54" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F55" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F56" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="7" t="n">
+      <c r="G56" s="7">
         <v>5</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>94</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="19" r="57" spans="1:12">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H57" s="7" t="s">
         <v>97</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D58" s="3" t="n"/>
-      <c r="E58" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F58" s="3" t="n"/>
-      <c r="G58" s="3" t="n"/>
-      <c r="H58" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>17</v>
@@ -1906,107 +1831,107 @@
       <c r="K58" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="L58" s="3" t="n"/>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H59" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H60" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H61" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H62" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H63" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H64" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H65" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D66" s="3" t="n"/>
+        <v>152</v>
+      </c>
+      <c r="D66" s="3"/>
       <c r="E66" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G66" s="3" t="n">
+        <v>147</v>
+      </c>
+      <c r="G66" s="3">
         <v>2</v>
       </c>
-      <c r="H66" s="3" t="n"/>
-      <c r="I66" s="2" t="n"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="2"/>
       <c r="J66" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="L66" s="3" t="s"/>
-    </row>
-    <row r="67" spans="1:12">
+        <v>138</v>
+      </c>
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F67" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G67" s="7" t="n">
+        <v>148</v>
+      </c>
+      <c r="G67" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F68" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G68" s="7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
+        <v>149</v>
+      </c>
+      <c r="G68" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F69" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>95</v>
@@ -2015,45 +1940,40 @@
         <v>90</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K40"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="2" style="7" width="12.1640625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="7" width="12.83203125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="28.1640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="12.83203125"/>
-    <col customWidth="1" max="9" min="9" style="7" width="30.6640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
-    <col customWidth="1" max="12" min="12" style="7" width="31.83203125"/>
-    <col customWidth="1" max="33" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="34" style="7" width="10.83203125"/>
+    <col min="1" max="1" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.83203125" style="7" customWidth="1"/>
+    <col min="13" max="34" width="10.83203125" style="7" customWidth="1"/>
+    <col min="35" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2070,13 +1990,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -2091,88 +2011,88 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="3" t="n"/>
+        <v>143</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+        <v>144</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="3" t="n"/>
+        <v>143</v>
+      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="3" t="n"/>
+        <v>143</v>
+      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="3" t="n"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2186,7 +2106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F7" s="7" t="s">
         <v>32</v>
       </c>
@@ -2197,13 +2117,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H8" s="7" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update example to fix CI failure.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="158">
   <si>
     <t>Run</t>
   </si>
@@ -512,6 +512,10 @@
   </si>
   <si>
     <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Safari/604.1.38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -912,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A43" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1724,7 +1728,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>122</v>
@@ -1885,7 +1889,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Avoid Travis CI failure.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -1,44 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/TestCases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="160">
   <si>
     <t>Run</t>
   </si>
@@ -515,74 +509,77 @@
   </si>
   <si>
     <t>AT.Login.13</t>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="11"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="DengXian"/>
+      <family val="4"/>
       <charset val="134"/>
-      <family val="4"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,41 +603,47 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
-    <cellStyle builtinId="8" hidden="1" name="超链接" xfId="1"/>
-    <cellStyle builtinId="9" hidden="1" name="已访问的超链接" xfId="2"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -906,36 +909,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="A47" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="7" width="6.5"/>
-    <col customWidth="1" max="2" min="2" style="7" width="18.1640625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="7" width="21.33203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="7" width="18"/>
-    <col customWidth="1" max="5" min="5" style="7" width="9"/>
-    <col customWidth="1" max="6" min="6" style="7" width="11"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="38.1640625"/>
-    <col customWidth="1" max="8" min="8" style="7" width="19"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="7" width="40"/>
-    <col customWidth="1" max="10" min="10" style="7" width="8.33203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="7" width="80.1640625"/>
-    <col customWidth="1" max="35" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="36" style="7" width="10.83203125"/>
+    <col min="1" max="1" width="6.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11" style="7" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" style="7" customWidth="1"/>
+    <col min="9" max="9" width="40" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="36" width="10.83203125" style="7" customWidth="1"/>
+    <col min="37" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -973,7 +972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -989,21 +988,21 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1019,8 +1018,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1033,14 +1032,14 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1048,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1064,8 +1063,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1078,9 +1077,9 @@
       <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="3" t="n"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D7" s="7" t="s">
         <v>31</v>
       </c>
@@ -1097,7 +1096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1108,7 +1107,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="7" t="s">
         <v>39</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F10" s="7" t="s">
         <v>32</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1149,8 +1148,8 @@
       <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="n"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1163,9 +1162,9 @@
       <c r="K11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="3" t="n"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="7" t="s">
         <v>46</v>
       </c>
@@ -1182,15 +1181,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F14" s="7" t="s">
         <v>32</v>
       </c>
@@ -1201,7 +1200,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -1217,8 +1216,8 @@
       <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1231,9 +1230,9 @@
       <c r="K15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L15" s="3" t="n"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="7" t="s">
         <v>55</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D17" s="7" t="s">
         <v>59</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D18" s="7" t="s">
         <v>62</v>
       </c>
@@ -1280,11 +1279,11 @@
       <c r="H18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D19" s="7" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1291,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
@@ -1308,8 +1307,8 @@
       <c r="E20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1322,9 +1321,9 @@
       <c r="K20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="3" t="n"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D21" s="7" t="s">
         <v>69</v>
       </c>
@@ -1337,11 +1336,11 @@
       <c r="H21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H22" s="7" t="s">
         <v>34</v>
       </c>
@@ -1349,7 +1348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D24" s="7" t="s">
         <v>71</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1387,12 +1386,12 @@
       <c r="C25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="3" t="n"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="n"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="2" t="s">
         <v>77</v>
       </c>
@@ -1405,9 +1404,9 @@
       <c r="K25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L25" s="3" t="n"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H26" s="7" t="s">
         <v>80</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -1425,12 +1424,12 @@
       <c r="C27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="3" t="n"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="3" t="n"/>
-      <c r="G27" s="3" t="n"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="2" t="s">
         <v>84</v>
       </c>
@@ -1443,9 +1442,9 @@
       <c r="K27" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L27" s="3" t="n"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H28" s="7" t="s">
         <v>80</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>49</v>
       </c>
@@ -1463,12 +1462,12 @@
       <c r="C29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="3" t="n"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F29" s="3" t="n"/>
-      <c r="G29" s="3" t="n"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="2" t="s">
         <v>88</v>
       </c>
@@ -1481,9 +1480,9 @@
       <c r="K29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="3" t="n"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H30" s="7" t="s">
         <v>80</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
@@ -1501,12 +1500,12 @@
       <c r="C31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="3" t="n"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="3" t="n"/>
-      <c r="G31" s="3" t="n"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="2" t="s">
         <v>91</v>
       </c>
@@ -1519,9 +1518,9 @@
       <c r="K31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L31" s="3" t="n"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H32" s="7" t="s">
         <v>80</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -1539,12 +1538,12 @@
       <c r="C33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="3" t="n"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="3" t="n"/>
-      <c r="G33" s="3" t="n"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="2" t="s">
         <v>95</v>
       </c>
@@ -1557,9 +1556,9 @@
       <c r="K33" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L33" s="3" t="n"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H34" s="7" t="s">
         <v>98</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -1577,7 +1576,7 @@
       <c r="C35" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="3" t="n"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="2" t="s">
         <v>94</v>
       </c>
@@ -1587,17 +1586,17 @@
       <c r="G35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H35" s="3" t="n"/>
-      <c r="I35" s="3" t="n"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
       <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L35" s="3" t="n"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F36" s="7" t="s">
         <v>104</v>
       </c>
@@ -1605,26 +1604,26 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="7" t="n">
+      <c r="G37" s="7">
         <v>2</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I38" s="7" t="n">
+      <c r="I38" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H39" s="7" t="s">
         <v>108</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H40" s="7" t="s">
         <v>109</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H41" s="7" t="s">
         <v>111</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
@@ -1658,25 +1657,25 @@
       <c r="C42" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="3" t="n"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="2" t="n"/>
-      <c r="H42" s="3" t="n"/>
-      <c r="I42" s="3" t="n"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
       <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L42" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="18" r="43" spans="1:12">
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="7" t="s">
         <v>116</v>
       </c>
@@ -1684,17 +1683,17 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F44" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F45" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F46" s="7" t="s">
         <v>120</v>
       </c>
@@ -1702,16 +1701,16 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F47" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F48" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G48" s="7" t="n">
+      <c r="G48" s="7">
         <v>5</v>
       </c>
       <c r="H48" s="4" t="s">
@@ -1721,12 +1720,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H49" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="50" spans="1:12">
+    <row r="50" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H50" s="7" t="s">
         <v>98</v>
       </c>
@@ -1734,9 +1733,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>125</v>
@@ -1744,25 +1743,25 @@
       <c r="C51" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D51" s="3" t="n"/>
+      <c r="D51" s="3"/>
       <c r="E51" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G51" s="2" t="n"/>
-      <c r="H51" s="3" t="n"/>
-      <c r="I51" s="3" t="n"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
       <c r="J51" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K51" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="L51" s="3" t="s"/>
-    </row>
-    <row customHeight="1" ht="18" r="52" spans="1:12">
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F52" s="7" t="s">
         <v>116</v>
       </c>
@@ -1770,17 +1769,17 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F53" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F54" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F55" s="7" t="s">
         <v>128</v>
       </c>
@@ -1788,16 +1787,16 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F56" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F57" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G57" s="7" t="n">
+      <c r="G57" s="7">
         <v>5</v>
       </c>
       <c r="H57" s="4" t="s">
@@ -1807,15 +1806,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H58" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I58" s="7" t="n">
+      <c r="I58" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H59" s="4" t="s">
         <v>131</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>129</v>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="60" spans="1:12">
+    <row r="60" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H60" s="7" t="s">
         <v>98</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>49</v>
       </c>
@@ -1841,12 +1840,12 @@
       <c r="C61" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D61" s="3" t="n"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F61" s="3" t="n"/>
-      <c r="G61" s="3" t="n"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
       <c r="H61" s="2" t="s">
         <v>136</v>
       </c>
@@ -1859,14 +1858,14 @@
       <c r="K61" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L61" s="3" t="n"/>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H62" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H63" s="7" t="s">
         <v>139</v>
       </c>
@@ -1874,12 +1873,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H64" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H65" s="7" t="s">
         <v>140</v>
       </c>
@@ -1887,7 +1886,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H66" s="7" t="s">
         <v>80</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H67" s="6" t="s">
         <v>142</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H68" s="7" t="s">
         <v>80</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>49</v>
       </c>
@@ -1921,43 +1920,43 @@
       <c r="C69" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D69" s="3" t="n"/>
+      <c r="D69" s="3"/>
       <c r="E69" s="2" t="s">
         <v>145</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G69" s="3" t="n">
+      <c r="G69" s="3">
         <v>2</v>
       </c>
-      <c r="H69" s="3" t="n"/>
-      <c r="I69" s="2" t="n"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="2"/>
       <c r="J69" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="L69" s="3" t="n"/>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="L69" s="3"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F70" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="G70" s="7" t="n">
+      <c r="G70" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F71" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G71" s="7" t="n">
+      <c r="G71" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F72" s="7" t="s">
         <v>150</v>
       </c>
@@ -1973,40 +1972,35 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K41"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="2" style="7" width="12.1640625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="7" width="12.83203125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="28.1640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="12.83203125"/>
-    <col customWidth="1" max="9" min="9" style="7" width="30.6640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
-    <col customWidth="1" max="12" min="12" style="7" width="31.83203125"/>
-    <col customWidth="1" max="34" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="35" style="7" width="10.83203125"/>
+    <col min="1" max="1" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.83203125" style="7" customWidth="1"/>
+    <col min="13" max="35" width="10.83203125" style="7" customWidth="1"/>
+    <col min="36" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -2054,21 +2048,21 @@
       <c r="C2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="3" t="n"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2078,28 +2072,28 @@
       <c r="C3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="3" t="n"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -2109,23 +2103,23 @@
       <c r="C5" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="3" t="n"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="3" t="n"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2139,7 +2133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F7" s="7" t="s">
         <v>32</v>
       </c>
@@ -2150,13 +2144,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H8" s="7" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Support multi value for post data.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="163">
   <si>
     <t>Run</t>
   </si>
@@ -385,9 +385,6 @@
     <t>user-agent</t>
   </si>
   <si>
-    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Safari/604.1.38</t>
-  </si>
-  <si>
     <t>&lt;/headers&gt;</t>
   </si>
   <si>
@@ -415,9 +412,6 @@
     <t>2017-10-15 23:44:34</t>
   </si>
   <si>
-    <t>Mozilla/5.0 (MSIE 10.0; Windows NT 6.1; Trident/5.0)</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -509,6 +503,26 @@
   </si>
   <si>
     <t>AT.Login.13</t>
+  </si>
+  <si>
+    <t>"closed"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Mozilla/5.0 (MSIE 10.0; Windows NT 6.1; Trident/5.0)"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"python"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Safari/604.1.38"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>n</t>
@@ -912,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1649,7 +1663,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>113</v>
@@ -1680,30 +1694,30 @@
         <v>116</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F44" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F45" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F46" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F47" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -1717,12 +1731,12 @@
         <v>95</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H49" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1730,15 +1744,15 @@
         <v>98</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>93</v>
@@ -1757,7 +1771,7 @@
         <v>17</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L51" s="3"/>
     </row>
@@ -1766,30 +1780,30 @@
         <v>116</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F53" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F54" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F55" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F56" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -1803,7 +1817,7 @@
         <v>95</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -1816,10 +1830,10 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H59" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1827,7 +1841,7 @@
         <v>98</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -1835,22 +1849,22 @@
         <v>49</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>17</v>
@@ -1862,28 +1876,28 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H62" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H63" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H64" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H65" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -1891,15 +1905,15 @@
         <v>80</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H67" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -1907,7 +1921,7 @@
         <v>80</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -1915,17 +1929,17 @@
         <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G69" s="3">
         <v>2</v>
@@ -1936,13 +1950,13 @@
         <v>17</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L69" s="3"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F70" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G70" s="7">
         <v>2</v>
@@ -1950,7 +1964,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F71" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G71" s="7">
         <v>1</v>
@@ -1958,7 +1972,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F72" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>96</v>
@@ -1967,7 +1981,7 @@
         <v>91</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2017,13 +2031,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -2043,14 +2057,14 @@
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -2067,10 +2081,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
@@ -2098,10 +2112,10 @@
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">

</xml_diff>

<commit_message>
Fix driver path for UI Engine.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -102,13 +102,23 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
   <si>
     <t>Run</t>
   </si>
@@ -161,27 +171,34 @@
     <t>open</t>
   </si>
   <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>2017-10-22 16:51:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Line 0] Message: '' executable may have wrong permissions. Please see https://sites.google.com/a/chromium.org/chromedriver/home
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>AT.UI.Home.02</t>
+  </si>
+  <si>
+    <t>Home(Custom URL)</t>
+  </si>
+  <si>
+    <t>Custom URL</t>
+  </si>
+  <si>
+    <t>http://www.baidu.com</t>
+  </si>
+  <si>
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-21 23:57:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
-    <t>AT.UI.Home.02</t>
-  </si>
-  <si>
-    <t>Home(Custom URL)</t>
-  </si>
-  <si>
-    <t>Custom URL</t>
-  </si>
-  <si>
-    <t>http://www.baidu.com</t>
-  </si>
-  <si>
     <t>2017-09-30 11:44:29</t>
   </si>
   <si>
@@ -200,9 +217,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-10-21 23:57:12</t>
-  </si>
-  <si>
     <t>Search box</t>
   </si>
   <si>
@@ -245,9 +259,6 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-10-21 23:57:15</t>
-  </si>
-  <si>
     <t>(Load the saved)</t>
   </si>
   <si>
@@ -453,9 +464,6 @@
   </si>
   <si>
     <t>headers{</t>
-  </si>
-  <si>
-    <t>2017-10-21 23:57:19</t>
   </si>
   <si>
     <t>user-agent</t>
@@ -1074,20 +1082,22 @@
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="n"/>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
@@ -1098,19 +1108,19 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L3" s="3" t="n"/>
     </row>
     <row r="4" spans="1:12">
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1118,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1126,13 +1136,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>15</v>
@@ -1143,67 +1153,69 @@
         <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="3" t="n"/>
+        <v>18</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="D7" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1211,13 +1223,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>15</v>
@@ -1228,15 +1240,17 @@
         <v>16</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="3" t="n"/>
+        <v>18</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="D12" s="7" t="s">
@@ -1246,13 +1260,13 @@
         <v>47</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1265,13 +1279,13 @@
     </row>
     <row r="14" spans="1:12">
       <c r="F14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1299,7 +1313,7 @@
         <v>53</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>54</v>
@@ -1317,7 +1331,7 @@
         <v>57</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>58</v>
@@ -1334,7 +1348,7 @@
         <v>60</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>61</v>
@@ -1359,10 +1373,10 @@
     </row>
     <row r="19" spans="1:12">
       <c r="D19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1390,7 +1404,7 @@
         <v>53</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>68</v>
@@ -1416,7 +1430,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="H22" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>70</v>
@@ -1433,7 +1447,7 @@
         <v>60</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>61</v>
@@ -1473,7 +1487,7 @@
         <v>78</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>79</v>
@@ -1511,7 +1525,7 @@
         <v>85</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>79</v>
@@ -1549,7 +1563,7 @@
         <v>89</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>79</v>
@@ -1587,7 +1601,7 @@
         <v>85</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>79</v>
@@ -1625,7 +1639,7 @@
         <v>96</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>97</v>
@@ -1663,7 +1677,7 @@
       <c r="H35" s="3" t="n"/>
       <c r="I35" s="3" t="n"/>
       <c r="J35" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>103</v>
@@ -1742,42 +1756,42 @@
       <c r="H42" s="3" t="n"/>
       <c r="I42" s="3" t="n"/>
       <c r="J42" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="L42" s="3" t="s"/>
     </row>
     <row customHeight="1" ht="18" r="43" spans="1:12">
       <c r="F43" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="F44" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="F45" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="F46" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G46" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="F47" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -1791,12 +1805,12 @@
         <v>95</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="H49" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row customHeight="1" ht="19" r="50" spans="1:12">
@@ -1804,7 +1818,7 @@
         <v>98</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -1812,7 +1826,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>93</v>
@@ -1828,42 +1842,42 @@
       <c r="H51" s="3" t="n"/>
       <c r="I51" s="3" t="n"/>
       <c r="J51" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L51" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="18" r="52" spans="1:12">
       <c r="F52" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="F53" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="F54" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="F55" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="F56" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -1877,7 +1891,7 @@
         <v>95</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -1890,10 +1904,10 @@
     </row>
     <row r="59" spans="1:12">
       <c r="H59" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I59" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="I59" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row customHeight="1" ht="19" r="60" spans="1:12">
@@ -1901,7 +1915,7 @@
         <v>98</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -1909,25 +1923,25 @@
         <v>49</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="D61" s="3" t="n"/>
       <c r="E61" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F61" s="3" t="n"/>
       <c r="G61" s="3" t="n"/>
       <c r="H61" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="J61" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K61" s="3" t="s">
         <v>103</v>
@@ -1936,28 +1950,28 @@
     </row>
     <row r="62" spans="1:12">
       <c r="H62" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="H63" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="H64" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="H65" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -1965,15 +1979,15 @@
         <v>80</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="H67" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -1981,7 +1995,7 @@
         <v>80</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -1989,17 +2003,17 @@
         <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D69" s="3" t="n"/>
       <c r="E69" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="G69" s="3" t="n">
         <v>2</v>
@@ -2007,16 +2021,16 @@
       <c r="H69" s="3" t="n"/>
       <c r="I69" s="2" t="n"/>
       <c r="J69" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L69" s="3" t="n"/>
     </row>
     <row r="70" spans="1:12">
       <c r="F70" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G70" s="7" t="n">
         <v>2</v>
@@ -2024,7 +2038,7 @@
     </row>
     <row r="71" spans="1:12">
       <c r="F71" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G71" s="7" t="n">
         <v>1</v>
@@ -2032,7 +2046,7 @@
     </row>
     <row r="72" spans="1:12">
       <c r="F72" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>96</v>
@@ -2041,7 +2055,7 @@
         <v>91</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2096,13 +2110,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -2122,14 +2136,14 @@
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="D2" s="3" t="n"/>
       <c r="E2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
@@ -2146,10 +2160,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
@@ -2161,7 +2175,7 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="n"/>
       <c r="K3" s="3" t="n"/>
@@ -2169,7 +2183,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2177,10 +2191,10 @@
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">
@@ -2192,7 +2206,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" s="3" t="n"/>
       <c r="K5" s="3" t="n"/>
@@ -2200,32 +2214,32 @@
     </row>
     <row r="6" spans="1:12">
       <c r="F6" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="H8" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more actions for UI Engine.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -1,144 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jia/Dropbox/v2test/TestCases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
-    <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Tests1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$41</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests1!$A$1:$K$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests2!$A$1:$K$8</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="163">
   <si>
     <t>Run</t>
   </si>
@@ -618,74 +512,85 @@
   </si>
   <si>
     <t>AT.Login.13</t>
+  </si>
+  <si>
+    <t>su</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_attribute.value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="DengXian"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="DengXian"/>
+      <family val="2"/>
       <charset val="134"/>
-      <family val="2"/>
-      <color theme="11"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="DengXian"/>
+      <family val="4"/>
       <charset val="134"/>
-      <family val="4"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,41 +614,47 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
-    <cellStyle builtinId="8" hidden="1" name="超链接" xfId="1"/>
-    <cellStyle builtinId="9" hidden="1" name="已访问的超链接" xfId="2"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1009,36 +920,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="A34" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="7" width="6.5"/>
-    <col customWidth="1" max="2" min="2" style="7" width="18.1640625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="7" width="21.33203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="7" width="18"/>
-    <col customWidth="1" max="5" min="5" style="7" width="9"/>
-    <col customWidth="1" max="6" min="6" style="7" width="11"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="38.1640625"/>
-    <col customWidth="1" max="8" min="8" style="7" width="19"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="7" width="40"/>
-    <col customWidth="1" max="10" min="10" style="7" width="8.33203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="7" width="80.1640625"/>
-    <col customWidth="1" max="36" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="37" style="7" width="10.83203125"/>
+    <col min="1" max="1" width="6.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11" style="7" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" style="7" customWidth="1"/>
+    <col min="9" max="9" width="40" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="37" width="10.83203125" style="7" customWidth="1"/>
+    <col min="38" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1092,21 +999,21 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1122,8 +1029,8 @@
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1136,14 +1043,14 @@
       <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1151,7 +1058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1167,8 +1074,8 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1181,9 +1088,9 @@
       <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="3" t="n"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D7" s="7" t="s">
         <v>31</v>
       </c>
@@ -1200,7 +1107,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1211,7 +1118,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="7" t="s">
         <v>39</v>
       </c>
@@ -1225,7 +1132,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F10" s="7" t="s">
         <v>32</v>
       </c>
@@ -1236,7 +1143,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1252,8 +1159,8 @@
       <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="n"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1266,9 +1173,9 @@
       <c r="K11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="3" t="n"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="7" t="s">
         <v>46</v>
       </c>
@@ -1285,260 +1192,232 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F14" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>40</v>
+        <v>160</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H15" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H16" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
-      <c r="H15" s="2" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L15" s="3" t="n"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="D16" s="7" t="s">
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D18" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="D17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="D18" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I20" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="D19" s="7" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
-      <c r="H20" s="2" t="s">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="3" t="n"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="D21" s="7" t="s">
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D23" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="H22" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="D23" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I25" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="D24" s="7" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D26" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H26" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I26" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="3" t="n"/>
-      <c r="E25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="n"/>
-      <c r="H25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L25" s="3" t="n"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="H26" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="3" t="n"/>
+        <v>75</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="3" t="n"/>
-      <c r="G27" s="3" t="n"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>17</v>
@@ -1546,9 +1425,9 @@
       <c r="K27" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L27" s="3" t="n"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H28" s="7" t="s">
         <v>80</v>
       </c>
@@ -1556,27 +1435,27 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="3" t="n"/>
+        <v>83</v>
+      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F29" s="3" t="n"/>
-      <c r="G29" s="3" t="n"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>17</v>
@@ -1584,9 +1463,9 @@
       <c r="K29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="3" t="n"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H30" s="7" t="s">
         <v>80</v>
       </c>
@@ -1594,7 +1473,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
@@ -1602,19 +1481,19 @@
         <v>86</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="3" t="n"/>
+        <v>87</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="3" t="n"/>
-      <c r="G31" s="3" t="n"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>17</v>
@@ -1622,9 +1501,9 @@
       <c r="K31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L31" s="3" t="n"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H32" s="7" t="s">
         <v>80</v>
       </c>
@@ -1632,381 +1511,403 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="3" t="n"/>
+        <v>90</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" s="3" t="n"/>
-      <c r="G33" s="3" t="n"/>
+        <v>76</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L33" s="3" t="n"/>
-    </row>
-    <row r="34" spans="1:12">
+        <v>79</v>
+      </c>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H34" s="7" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="3" t="n"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H35" s="3" t="n"/>
-      <c r="I35" s="3" t="n"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H36" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L35" s="3" t="n"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="F36" s="7" t="s">
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F38" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
-      <c r="F37" s="7" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F39" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="7" t="n">
+      <c r="G39" s="7">
         <v>2</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="H38" s="7" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H40" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I38" s="7" t="n">
+      <c r="I40" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="H39" s="7" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H41" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I39" s="7" t="b">
+      <c r="I41" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
-      <c r="H40" s="7" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H42" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I42" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
-      <c r="H41" s="7" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H43" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I43" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="2" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="3" t="n"/>
-      <c r="E42" s="2" t="s">
+      <c r="D44" s="3"/>
+      <c r="E44" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="2" t="n"/>
-      <c r="H42" s="3" t="n"/>
-      <c r="I42" s="3" t="n"/>
-      <c r="J42" s="3" t="s">
+      <c r="G44" s="2"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="K44" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L42" s="3" t="s"/>
-    </row>
-    <row customHeight="1" ht="18" r="43" spans="1:12">
-      <c r="F43" s="7" t="s">
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F45" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
-      <c r="F44" s="7" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F46" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
-      <c r="F45" s="7" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F47" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
-      <c r="F46" s="7" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F48" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G48" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
-      <c r="F47" s="7" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F49" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
-      <c r="F48" s="7" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F50" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G48" s="7" t="n">
+      <c r="G50" s="7">
         <v>5</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I50" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
-      <c r="H49" s="4" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H51" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="50" spans="1:12">
-      <c r="H50" s="7" t="s">
+    <row r="52" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H52" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="2" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D51" s="3" t="n"/>
-      <c r="E51" s="2" t="s">
+      <c r="D53" s="3"/>
+      <c r="E53" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G51" s="2" t="n"/>
-      <c r="H51" s="3" t="n"/>
-      <c r="I51" s="3" t="n"/>
-      <c r="J51" s="3" t="s">
+      <c r="G53" s="2"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K51" s="3" t="s">
+      <c r="K53" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="L51" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="18" r="52" spans="1:12">
-      <c r="F52" s="7" t="s">
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F54" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G54" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
-      <c r="F53" s="7" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F55" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
-      <c r="F54" s="7" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F56" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
-      <c r="F55" s="7" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F57" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G57" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
-      <c r="F56" s="7" t="s">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F58" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
-      <c r="F57" s="7" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F59" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G57" s="7" t="n">
+      <c r="G59" s="7">
         <v>5</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I57" s="7" t="s">
+      <c r="I59" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
-      <c r="H58" s="4" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H60" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I58" s="7" t="n">
+      <c r="I60" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
-      <c r="H59" s="4" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H61" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I61" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="60" spans="1:12">
-      <c r="H60" s="7" t="s">
+    <row r="62" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H62" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I62" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
-      <c r="A61" s="2" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D61" s="3" t="n"/>
-      <c r="E61" s="2" t="s">
+      <c r="D63" s="3"/>
+      <c r="E63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F61" s="3" t="n"/>
-      <c r="G61" s="3" t="n"/>
-      <c r="H61" s="2" t="s">
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J61" s="3" t="s">
+      <c r="J63" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="K63" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L61" s="3" t="n"/>
-    </row>
-    <row r="62" spans="1:12">
-      <c r="H62" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
-      <c r="H63" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="I63" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="L63" s="3"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H64" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H65" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H66" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
-      <c r="H67" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H67" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H68" s="7" t="s">
         <v>80</v>
       </c>
@@ -2014,102 +1915,113 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H69" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H70" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="3" t="n"/>
-      <c r="E69" s="2" t="s">
+      <c r="D71" s="3"/>
+      <c r="E71" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F71" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G69" s="3" t="n">
+      <c r="G71" s="3">
         <v>2</v>
       </c>
-      <c r="H69" s="3" t="n"/>
-      <c r="I69" s="2" t="n"/>
-      <c r="J69" s="3" t="s">
+      <c r="H71" s="3"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K69" s="3" t="s">
+      <c r="K71" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L69" s="3" t="n"/>
-    </row>
-    <row r="70" spans="1:12">
-      <c r="F70" s="7" t="s">
+      <c r="L71" s="3"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F72" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G70" s="7" t="n">
+      <c r="G72" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
-      <c r="F71" s="7" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F73" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G71" s="7" t="n">
+      <c r="G73" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
-      <c r="F72" s="7" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F74" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G72" s="7" t="s">
+      <c r="G74" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H72" s="7" t="s">
+      <c r="H74" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I72" s="7" t="s">
+      <c r="I74" s="7" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K41"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <autoFilter ref="A1:K43"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="2" style="7" width="12.1640625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="7" width="12.83203125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="7" width="28.1640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="7" width="12.83203125"/>
-    <col customWidth="1" max="9" min="9" style="7" width="30.6640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="7" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="7" width="19.6640625"/>
-    <col customWidth="1" max="12" min="12" style="7" width="31.83203125"/>
-    <col customWidth="1" max="35" min="13" style="7" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="36" style="7" width="10.83203125"/>
+    <col min="1" max="1" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.83203125" style="7" customWidth="1"/>
+    <col min="13" max="36" width="10.83203125" style="7" customWidth="1"/>
+    <col min="37" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2147,7 +2059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -2157,21 +2069,21 @@
       <c r="C2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="3" t="n"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="3" t="n"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2181,28 +2093,28 @@
       <c r="C3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="3" t="n"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="3" t="n"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -2212,23 +2124,23 @@
       <c r="C5" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="3" t="n"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="3" t="n"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2242,7 +2154,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F7" s="7" t="s">
         <v>32</v>
       </c>
@@ -2253,13 +2165,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H8" s="7" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K8"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use bing instead of baidu in example to fix connection issues.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="162">
   <si>
     <t>Run</t>
   </si>
@@ -84,7 +84,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-10-22 22:04:50</t>
+    <t>2017-10-22 23:31:22</t>
   </si>
   <si>
     <t>n</t>
@@ -99,415 +99,421 @@
     <t>Custom URL</t>
   </si>
   <si>
+    <t>http://www.bing.com</t>
+  </si>
+  <si>
+    <t>2017-09-30 11:44:29</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.01</t>
+  </si>
+  <si>
+    <t>Search(Save element)</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>2017-10-22 23:31:24</t>
+  </si>
+  <si>
+    <t>Search box</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>sb_form_q</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>(Save element)</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>searchbox</t>
+  </si>
+  <si>
+    <t>Search btn</t>
+  </si>
+  <si>
+    <t>sb_form_go</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>AT.UI.Search.02</t>
+  </si>
+  <si>
+    <t>Search(Load the saved)</t>
+  </si>
+  <si>
+    <t>2017-10-22 23:31:29</t>
+  </si>
+  <si>
+    <t>(Load the saved)</t>
+  </si>
+  <si>
+    <t>saved</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>get_attribute.value</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>AT.UI.Login.01</t>
+  </si>
+  <si>
+    <t>Login(Click)</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>https://www.v2ex.com/signin</t>
+  </si>
+  <si>
+    <t>2017-09-30 11:44:42</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//input[@type='text' and @class='sl']</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>//input[@type='password' and @class='sl']</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Submit (waitting)</t>
+  </si>
+  <si>
+    <t>//input[@type='submit']</t>
+  </si>
+  <si>
+    <t>waiting</t>
+  </si>
+  <si>
+    <t>AT.UI.Login.02</t>
+  </si>
+  <si>
+    <t>Login(Press)</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>2017-09-25 19:29:57</t>
+  </si>
+  <si>
+    <t>Username (waiting)</t>
+  </si>
+  <si>
+    <t>deepjia</t>
+  </si>
+  <si>
+    <t>press RETURN</t>
+  </si>
+  <si>
+    <t>press</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>AT.BG.Shell.01</t>
+  </si>
+  <si>
+    <t>Shell Command</t>
+  </si>
+  <si>
+    <t>shell</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>ls -l</t>
+  </si>
+  <si>
+    <t>2017-10-02 19:46:35</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>config.ini</t>
+  </si>
+  <si>
+    <t>AT.BG.Shell.02</t>
+  </si>
+  <si>
+    <t>Bash Script</t>
+  </si>
+  <si>
+    <t>bash</t>
+  </si>
+  <si>
+    <t>Example.sh</t>
+  </si>
+  <si>
+    <t>AT.BG.Shell.03</t>
+  </si>
+  <si>
+    <t>Python Script</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>Example.py</t>
+  </si>
+  <si>
+    <t>Executable File</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.01</t>
+  </si>
+  <si>
+    <t>Get Request</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>https://api.github.com</t>
+  </si>
+  <si>
+    <t>2017-10-09 22:02:18</t>
+  </si>
+  <si>
+    <t>in.text</t>
+  </si>
+  <si>
+    <t>emojis</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.02</t>
+  </si>
+  <si>
+    <t>headers</t>
+  </si>
+  <si>
+    <t>{'user-agent': 'my-app/0.0.1'}</t>
+  </si>
+  <si>
+    <t>2017-10-03 23:39:35</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>{'key1': 'value1', 'key2': 'value2'}</t>
+  </si>
+  <si>
+    <t>timeout</t>
+  </si>
+  <si>
+    <t>equal.status_code</t>
+  </si>
+  <si>
+    <t>equal.ok</t>
+  </si>
+  <si>
+    <t>!in.text</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>!equal.text</t>
+  </si>
+  <si>
+    <t>zzzz</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.03</t>
+  </si>
+  <si>
+    <t>headers{</t>
+  </si>
+  <si>
+    <t>2017-10-22 23:31:34</t>
+  </si>
+  <si>
+    <t>user-agent</t>
+  </si>
+  <si>
+    <t>"Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Safari/604.1.38"</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>params{</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>"python"</t>
+  </si>
+  <si>
+    <t>https://www.v2ex.com/api/nodes/show.json</t>
+  </si>
+  <si>
+    <t>log.text</t>
+  </si>
+  <si>
+    <t>Django</t>
+  </si>
+  <si>
+    <t>AT.HTTP.Get.04</t>
+  </si>
+  <si>
+    <t>2017-10-15 23:44:34</t>
+  </si>
+  <si>
+    <t>"Mozilla/5.0 (MSIE 10.0; Windows NT 6.1; Trident/5.0)"</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>"closed"</t>
+  </si>
+  <si>
+    <t>https://api.github.com/repos/txels/ddt/issues</t>
+  </si>
+  <si>
+    <t>equal.json.0.state</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Add zeros</t>
+  </si>
+  <si>
+    <t>AT.MYSQL.Select.01</t>
+  </si>
+  <si>
+    <t>DB Test</t>
+  </si>
+  <si>
+    <t>mysql</t>
+  </si>
+  <si>
+    <t>fetchone</t>
+  </si>
+  <si>
+    <t>SELECT name FROM help_keyword;</t>
+  </si>
+  <si>
+    <t>fetchone.name</t>
+  </si>
+  <si>
+    <t>fetchall</t>
+  </si>
+  <si>
+    <t>AES_ENCRYPT</t>
+  </si>
+  <si>
+    <t>fetchmany.5</t>
+  </si>
+  <si>
+    <t>AT.Locust.01</t>
+  </si>
+  <si>
+    <t>Load Test</t>
+  </si>
+  <si>
+    <t>locust</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+  </si>
+  <si>
+    <t>2017-10-09 22:02:22</t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>HOST</t>
+  </si>
+  <si>
+    <t>LocustExample.py</t>
+  </si>
+  <si>
+    <t>Locate/Encapsulate</t>
+  </si>
+  <si>
+    <t>Action/Check</t>
+  </si>
+  <si>
+    <t>AT.Login.11</t>
+  </si>
+  <si>
+    <t>登录</t>
+  </si>
+  <si>
+    <t>uI</t>
+  </si>
+  <si>
+    <t>AT.Login.12</t>
+  </si>
+  <si>
     <t>http://www.baidu.com</t>
   </si>
   <si>
-    <t>2017-09-30 11:44:29</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>http://www.bing.com</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.01</t>
-  </si>
-  <si>
-    <t>Search(Save element)</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>2017-10-22 22:04:59</t>
-  </si>
-  <si>
-    <t>Search box</t>
-  </si>
-  <si>
-    <t>id</t>
+    <t>AT.Login.13</t>
   </si>
   <si>
     <t>kw</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>(Save element)</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>searchbox</t>
-  </si>
-  <si>
-    <t>Search btn</t>
-  </si>
-  <si>
     <t>su</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>find</t>
-  </si>
-  <si>
-    <t>AT.UI.Search.02</t>
-  </si>
-  <si>
-    <t>Search(Load the saved)</t>
-  </si>
-  <si>
-    <t>2017-10-22 22:05:02</t>
-  </si>
-  <si>
-    <t>(Load the saved)</t>
-  </si>
-  <si>
-    <t>saved</t>
-  </si>
-  <si>
-    <t>wait</t>
-  </si>
-  <si>
-    <t>get_attribute.value</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>AT.UI.Login.01</t>
-  </si>
-  <si>
-    <t>Login(Click)</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>https://www.v2ex.com/signin</t>
-  </si>
-  <si>
-    <t>2017-09-30 11:44:42</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>//input[@type='text' and @class='sl']</t>
-  </si>
-  <si>
-    <t>aaaaa</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>//input[@type='password' and @class='sl']</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Submit (waitting)</t>
-  </si>
-  <si>
-    <t>//input[@type='submit']</t>
-  </si>
-  <si>
-    <t>waiting</t>
-  </si>
-  <si>
-    <t>AT.UI.Login.02</t>
-  </si>
-  <si>
-    <t>Login(Press)</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>2017-09-25 19:29:57</t>
-  </si>
-  <si>
-    <t>Username (waiting)</t>
-  </si>
-  <si>
-    <t>deepjia</t>
-  </si>
-  <si>
-    <t>press RETURN</t>
-  </si>
-  <si>
-    <t>press</t>
-  </si>
-  <si>
-    <t>RETURN</t>
-  </si>
-  <si>
-    <t>AT.BG.Shell.01</t>
-  </si>
-  <si>
-    <t>Shell Command</t>
-  </si>
-  <si>
-    <t>shell</t>
-  </si>
-  <si>
-    <t>command</t>
-  </si>
-  <si>
-    <t>ls -l</t>
-  </si>
-  <si>
-    <t>2017-10-02 19:46:35</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>config.ini</t>
-  </si>
-  <si>
-    <t>AT.BG.Shell.02</t>
-  </si>
-  <si>
-    <t>Bash Script</t>
-  </si>
-  <si>
-    <t>bash</t>
-  </si>
-  <si>
-    <t>Example.sh</t>
-  </si>
-  <si>
-    <t>AT.BG.Shell.03</t>
-  </si>
-  <si>
-    <t>Python Script</t>
-  </si>
-  <si>
-    <t>python</t>
-  </si>
-  <si>
-    <t>Example.py</t>
-  </si>
-  <si>
-    <t>Executable File</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.01</t>
-  </si>
-  <si>
-    <t>Get Request</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
-    <t>get</t>
-  </si>
-  <si>
-    <t>https://api.github.com</t>
-  </si>
-  <si>
-    <t>2017-10-09 22:02:18</t>
-  </si>
-  <si>
-    <t>in.text</t>
-  </si>
-  <si>
-    <t>emojis</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.02</t>
-  </si>
-  <si>
-    <t>headers</t>
-  </si>
-  <si>
-    <t>{'user-agent': 'my-app/0.0.1'}</t>
-  </si>
-  <si>
-    <t>2017-10-03 23:39:35</t>
-  </si>
-  <si>
-    <t>params</t>
-  </si>
-  <si>
-    <t>{'key1': 'value1', 'key2': 'value2'}</t>
-  </si>
-  <si>
-    <t>timeout</t>
-  </si>
-  <si>
-    <t>equal.status_code</t>
-  </si>
-  <si>
-    <t>equal.ok</t>
-  </si>
-  <si>
-    <t>!in.text</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>!equal.text</t>
-  </si>
-  <si>
-    <t>zzzz</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.03</t>
-  </si>
-  <si>
-    <t>headers{</t>
-  </si>
-  <si>
-    <t>2017-10-22 22:05:06</t>
-  </si>
-  <si>
-    <t>user-agent</t>
-  </si>
-  <si>
-    <t>"Mozilla/5.0 (Macintosh; Intel Mac OS X 10_12_6) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Safari/604.1.38"</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>params{</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>"python"</t>
-  </si>
-  <si>
-    <t>https://www.v2ex.com/api/nodes/show.json</t>
-  </si>
-  <si>
-    <t>log.text</t>
-  </si>
-  <si>
-    <t>Django</t>
-  </si>
-  <si>
-    <t>AT.HTTP.Get.04</t>
-  </si>
-  <si>
-    <t>2017-10-15 23:44:34</t>
-  </si>
-  <si>
-    <t>"Mozilla/5.0 (MSIE 10.0; Windows NT 6.1; Trident/5.0)"</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>"closed"</t>
-  </si>
-  <si>
-    <t>https://api.github.com/repos/txels/ddt/issues</t>
-  </si>
-  <si>
-    <t>equal.json.0.state</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>Add zeros</t>
-  </si>
-  <si>
-    <t>AT.MYSQL.Select.01</t>
-  </si>
-  <si>
-    <t>DB Test</t>
-  </si>
-  <si>
-    <t>mysql</t>
-  </si>
-  <si>
-    <t>fetchone</t>
-  </si>
-  <si>
-    <t>SELECT name FROM help_keyword;</t>
-  </si>
-  <si>
-    <t>fetchone.name</t>
-  </si>
-  <si>
-    <t>fetchall</t>
-  </si>
-  <si>
-    <t>AES_ENCRYPT</t>
-  </si>
-  <si>
-    <t>fetchmany.5</t>
-  </si>
-  <si>
-    <t>AT.Locust.01</t>
-  </si>
-  <si>
-    <t>Load Test</t>
-  </si>
-  <si>
-    <t>locust</t>
-  </si>
-  <si>
-    <t>CLIENT</t>
-  </si>
-  <si>
-    <t>2017-10-09 22:02:22</t>
-  </si>
-  <si>
-    <t>RATE</t>
-  </si>
-  <si>
-    <t>NUMBER</t>
-  </si>
-  <si>
-    <t>HOST</t>
-  </si>
-  <si>
-    <t>LocustExample.py</t>
-  </si>
-  <si>
-    <t>Locate/Encapsulate</t>
-  </si>
-  <si>
-    <t>Action/Check</t>
-  </si>
-  <si>
-    <t>AT.Login.11</t>
-  </si>
-  <si>
-    <t>登录</t>
-  </si>
-  <si>
-    <t>uI</t>
-  </si>
-  <si>
-    <t>AT.Login.12</t>
-  </si>
-  <si>
-    <t>AT.Login.13</t>
   </si>
 </sst>
 </file>
@@ -907,7 +913,7 @@
   <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView showRuler="0" tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125">
-      <selection activeCell="B7" sqref="B7:G7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -1038,7 +1044,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1046,13 +1052,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>15</v>
@@ -1069,61 +1075,61 @@
         <v>17</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="3" t="n"/>
     </row>
     <row r="7" spans="1:12">
       <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="D8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1131,13 +1137,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>15</v>
@@ -1154,30 +1160,30 @@
         <v>17</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L11" s="3" t="n"/>
     </row>
     <row r="12" spans="1:12">
       <c r="D12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="G12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="H13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I13" s="7" t="n">
         <v>1</v>
@@ -1185,23 +1191,29 @@
     </row>
     <row r="14" spans="1:12">
       <c r="F14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="15" spans="1:12">
+      <c r="F15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="H15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="H16" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1209,13 +1221,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>15</v>
@@ -1226,62 +1238,62 @@
         <v>16</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L17" s="3" t="n"/>
     </row>
     <row r="18" spans="1:12">
       <c r="D18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="D19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="D20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="I20" s="7" t="n">
         <v>5</v>
@@ -1289,10 +1301,10 @@
     </row>
     <row r="21" spans="1:12">
       <c r="D21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1300,13 +1312,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>15</v>
@@ -1317,28 +1329,28 @@
         <v>16</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L22" s="3" t="n"/>
     </row>
     <row r="23" spans="1:12">
       <c r="D23" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="H23" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I23" s="7" t="n">
         <v>5</v>
@@ -1346,38 +1358,38 @@
     </row>
     <row r="24" spans="1:12">
       <c r="H24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="D25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="7" t="s">
+      <c r="H25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="D26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="I26" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1385,37 +1397,37 @@
         <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D27" s="3" t="n"/>
       <c r="E27" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
       <c r="H27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L27" s="3" t="n"/>
     </row>
     <row r="28" spans="1:12">
       <c r="H28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1423,37 +1435,37 @@
         <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D29" s="3" t="n"/>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
       <c r="H29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L29" s="3" t="n"/>
     </row>
     <row r="30" spans="1:12">
       <c r="H30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1461,37 +1473,37 @@
         <v>19</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="D31" s="3" t="n"/>
       <c r="E31" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L31" s="3" t="n"/>
     </row>
     <row r="32" spans="1:12">
       <c r="H32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1499,37 +1511,37 @@
         <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D33" s="3" t="n"/>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L33" s="3" t="n"/>
     </row>
     <row r="34" spans="1:12">
       <c r="H34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1537,37 +1549,37 @@
         <v>19</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="D35" s="3" t="n"/>
       <c r="E35" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L35" s="3" t="n"/>
     </row>
     <row r="36" spans="1:12">
       <c r="H36" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1575,20 +1587,20 @@
         <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37" s="3" t="n"/>
       <c r="E37" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="H37" s="3" t="n"/>
       <c r="I37" s="3" t="n"/>
@@ -1596,32 +1608,32 @@
         <v>17</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L37" s="3" t="n"/>
     </row>
     <row r="38" spans="1:12">
       <c r="F38" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="F39" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G39" s="7" t="n">
         <v>2</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="H40" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I40" s="7" t="n">
         <v>200</v>
@@ -1629,7 +1641,7 @@
     </row>
     <row r="41" spans="1:12">
       <c r="H41" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I41" s="7" t="b">
         <v>1</v>
@@ -1637,18 +1649,18 @@
     </row>
     <row r="42" spans="1:12">
       <c r="H42" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="H43" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -1656,17 +1668,17 @@
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" s="3" t="n"/>
       <c r="E44" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G44" s="2" t="n"/>
       <c r="H44" s="3" t="n"/>
@@ -1675,66 +1687,66 @@
         <v>17</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L44" s="3" t="s"/>
     </row>
     <row customHeight="1" ht="18" r="45" spans="1:12">
       <c r="F45" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="F46" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="F47" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="F48" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="F49" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="F50" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G50" s="7" t="n">
         <v>5</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="H51" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row customHeight="1" ht="19" r="52" spans="1:12">
       <c r="H52" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -1742,17 +1754,17 @@
         <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="3" t="n"/>
       <c r="E53" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G53" s="2" t="n"/>
       <c r="H53" s="3" t="n"/>
@@ -1761,58 +1773,58 @@
         <v>17</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L53" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="18" r="54" spans="1:12">
       <c r="F54" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="F55" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="F56" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="F57" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="F58" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="F59" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G59" s="7" t="n">
         <v>5</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="H60" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I60" s="7" t="n">
         <v>200</v>
@@ -1820,18 +1832,18 @@
     </row>
     <row r="61" spans="1:12">
       <c r="H61" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I61" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="I61" s="7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row customHeight="1" ht="19" r="62" spans="1:12">
       <c r="H62" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -1839,79 +1851,79 @@
         <v>19</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="D63" s="3" t="n"/>
       <c r="E63" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F63" s="3" t="n"/>
       <c r="G63" s="3" t="n"/>
       <c r="H63" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L63" s="3" t="n"/>
     </row>
     <row r="64" spans="1:12">
       <c r="H64" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="H65" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="H66" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="H67" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="H68" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="H69" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="H70" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -1919,17 +1931,17 @@
         <v>19</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D71" s="3" t="n"/>
       <c r="E71" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="G71" s="3" t="n">
         <v>2</v>
@@ -1940,13 +1952,13 @@
         <v>17</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L71" s="3" t="n"/>
     </row>
     <row r="72" spans="1:12">
       <c r="F72" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G72" s="7" t="n">
         <v>2</v>
@@ -1954,7 +1966,7 @@
     </row>
     <row r="73" spans="1:12">
       <c r="F73" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G73" s="7" t="n">
         <v>1</v>
@@ -1962,16 +1974,16 @@
     </row>
     <row r="74" spans="1:12">
       <c r="F74" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I74" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I74" s="7" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2026,13 +2038,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -2052,14 +2064,14 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="D2" s="3" t="n"/>
       <c r="E2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
@@ -2076,10 +2088,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="3" t="n"/>
       <c r="E3" s="2" t="s">
@@ -2091,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="J3" s="3" t="n"/>
       <c r="K3" s="3" t="n"/>
@@ -2110,7 +2122,7 @@
         <v>159</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="3" t="n"/>
       <c r="E5" s="2" t="s">
@@ -2122,7 +2134,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="J5" s="3" t="n"/>
       <c r="K5" s="3" t="n"/>
@@ -2130,27 +2142,27 @@
     </row>
     <row r="6" spans="1:12">
       <c r="F6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Use Firefox in Travis CI..
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -3,13 +3,33 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Tests1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Tests2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
@@ -94,7 +114,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2017-12-02 11:04:16</t>
+    <t>2018-04-10 21:54:28</t>
   </si>
   <si>
     <t>n</t>
@@ -127,7 +147,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2017-12-02 11:04:28</t>
+    <t>2018-04-10 21:54:31</t>
   </si>
   <si>
     <t>Search box</t>
@@ -172,7 +192,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2017-12-02 11:04:38</t>
+    <t>2018-04-10 21:54:35</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -385,7 +405,7 @@
     <t>headers{</t>
   </si>
   <si>
-    <t>2017-12-02 11:04:47</t>
+    <t>2018-04-10 21:54:40</t>
   </si>
   <si>
     <t>user-agent</t>

</xml_diff>

<commit_message>
Use Headless Chrome in Travis CI.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -52,6 +52,16 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -114,7 +124,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2018-04-10 21:54:28</t>
+    <t>2018-04-10 22:42:47</t>
   </si>
   <si>
     <t>n</t>
@@ -147,7 +157,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2018-04-10 21:54:31</t>
+    <t>2018-04-10 22:42:50</t>
   </si>
   <si>
     <t>Search box</t>
@@ -192,7 +202,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2018-04-10 21:54:35</t>
+    <t>2018-04-10 22:42:53</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -405,7 +415,7 @@
     <t>headers{</t>
   </si>
   <si>
-    <t>2018-04-10 21:54:40</t>
+    <t>2018-04-10 22:42:58</t>
   </si>
   <si>
     <t>user-agent</t>

</xml_diff>

<commit_message>
Support Headless Mode for Chrome and Firefox.
</commit_message>
<xml_diff>
--- a/TestCases/Example.xlsx
+++ b/TestCases/Example.xlsx
@@ -62,6 +62,66 @@
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tests1!$A$1:$K$43</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Tests2!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -124,7 +184,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>2018-04-10 22:42:47</t>
+    <t>2018-04-11 00:19:12</t>
   </si>
   <si>
     <t>n</t>
@@ -157,7 +217,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>2018-04-10 22:42:50</t>
+    <t>2018-04-11 00:19:16</t>
   </si>
   <si>
     <t>Search box</t>
@@ -202,7 +262,7 @@
     <t>Search(Load the saved)</t>
   </si>
   <si>
-    <t>2018-04-10 22:42:53</t>
+    <t>2018-04-11 00:19:21</t>
   </si>
   <si>
     <t>(Load the saved)</t>
@@ -415,7 +475,7 @@
     <t>headers{</t>
   </si>
   <si>
-    <t>2018-04-10 22:42:58</t>
+    <t>2018-04-11 00:19:27</t>
   </si>
   <si>
     <t>user-agent</t>

</xml_diff>